<commit_message>
starting to build field lines from density
</commit_message>
<xml_diff>
--- a/resources/Test_Simulationen_2.xlsx
+++ b/resources/Test_Simulationen_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Programme\Physics-Capacitor-Simualtion\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DB82E4-748D-4124-8816-D21CC4FC534E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C1BD43-0B27-474E-9034-5909A2ED0DA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -63,9 +63,6 @@
     <t>num_field_lines</t>
   </si>
   <si>
-    <t>Test_0_002_d_16</t>
-  </si>
-  <si>
     <t>0.01</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
   </si>
   <si>
     <t>0.001</t>
-  </si>
-  <si>
-    <t>0.002</t>
   </si>
   <si>
     <t>False</t>
@@ -408,20 +402,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" customWidth="1"/>
-    <col min="12" max="12" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,117 +453,79 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="B2">
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
         <v>16</v>
-      </c>
-      <c r="C2">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
       </c>
       <c r="L2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4">
-        <v>16</v>
-      </c>
-      <c r="C4">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4">
         <v>51</v>
       </c>
     </row>

</xml_diff>